<commit_message>
Refactor capacitor table and add a capacitor
</commit_message>
<xml_diff>
--- a/library/Database_Students.xlsx
+++ b/library/Database_Students.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Александра\Documents\GitHub\Altium_BEng\library\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chern_000\Documents\Altium\Library\Altium_BEng\library\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62606BEA-9125-449B-88A5-7819C7D098EB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="7" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Резисторы" sheetId="1" r:id="rId1"/>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1000" uniqueCount="459">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1016" uniqueCount="464">
   <si>
     <t>ID</t>
   </si>
@@ -1760,11 +1759,26 @@
   <si>
     <t>https://www.ftdichip.com/Products/ICs/FT232R.htm</t>
   </si>
+  <si>
+    <t>Конденсатор чип 0603 0,22 мкФ 10 В ±5 %</t>
+  </si>
+  <si>
+    <t>CC0603JRX7R6BB224</t>
+  </si>
+  <si>
+    <t>Producer</t>
+  </si>
+  <si>
+    <t>pdf</t>
+  </si>
+  <si>
+    <t>Backup Help URL</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1883,7 +1897,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1946,6 +1960,9 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2227,7 +2244,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q30"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
@@ -3061,20 +3078,20 @@
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="Q3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="Q4" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="Q12" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="Q10" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="Q9" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="Q5" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="Q7" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="Q13" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="Q8" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="Q6" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="Q11" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="Q2" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="Q15" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="Q14" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="Q3" r:id="rId1"/>
+    <hyperlink ref="Q4" r:id="rId2"/>
+    <hyperlink ref="Q12" r:id="rId3"/>
+    <hyperlink ref="Q10" r:id="rId4"/>
+    <hyperlink ref="Q9" r:id="rId5"/>
+    <hyperlink ref="Q5" r:id="rId6"/>
+    <hyperlink ref="Q7" r:id="rId7"/>
+    <hyperlink ref="Q13" r:id="rId8"/>
+    <hyperlink ref="Q8" r:id="rId9"/>
+    <hyperlink ref="Q6" r:id="rId10"/>
+    <hyperlink ref="Q11" r:id="rId11"/>
+    <hyperlink ref="Q2" r:id="rId12"/>
+    <hyperlink ref="Q15" r:id="rId13"/>
+    <hyperlink ref="Q14" r:id="rId14"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId15"/>
@@ -3082,10 +3099,10 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
@@ -3518,16 +3535,16 @@
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="L2" r:id="rId1" xr:uid="{00000000-0004-0000-0900-000000000000}"/>
-    <hyperlink ref="L3" r:id="rId2" xr:uid="{00000000-0004-0000-0900-000001000000}"/>
-    <hyperlink ref="L4" r:id="rId3" xr:uid="{00000000-0004-0000-0900-000002000000}"/>
-    <hyperlink ref="L6" r:id="rId4" location="product-samplebuy" xr:uid="{00000000-0004-0000-0900-000003000000}"/>
-    <hyperlink ref="L5" r:id="rId5" xr:uid="{00000000-0004-0000-0900-000004000000}"/>
-    <hyperlink ref="L9" r:id="rId6" xr:uid="{00000000-0004-0000-0900-000005000000}"/>
-    <hyperlink ref="L8" r:id="rId7" xr:uid="{00000000-0004-0000-0900-000006000000}"/>
-    <hyperlink ref="L10" r:id="rId8" xr:uid="{00000000-0004-0000-0900-000007000000}"/>
-    <hyperlink ref="L7" r:id="rId9" location="product-documentation" xr:uid="{E551D280-D17E-4C5C-879A-3CDF56256191}"/>
-    <hyperlink ref="L11" r:id="rId10" xr:uid="{B5BF2EFD-3C64-46DF-AACD-718A648A07EE}"/>
+    <hyperlink ref="L2" r:id="rId1"/>
+    <hyperlink ref="L3" r:id="rId2"/>
+    <hyperlink ref="L4" r:id="rId3"/>
+    <hyperlink ref="L6" r:id="rId4" location="product-samplebuy"/>
+    <hyperlink ref="L5" r:id="rId5"/>
+    <hyperlink ref="L9" r:id="rId6"/>
+    <hyperlink ref="L8" r:id="rId7"/>
+    <hyperlink ref="L10" r:id="rId8"/>
+    <hyperlink ref="L7" r:id="rId9" location="product-documentation"/>
+    <hyperlink ref="L11" r:id="rId10"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId11"/>
@@ -3535,7 +3552,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -3753,11 +3770,11 @@
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="K3" r:id="rId1" xr:uid="{00000000-0004-0000-0A00-000000000000}"/>
-    <hyperlink ref="K4" r:id="rId2" xr:uid="{00000000-0004-0000-0A00-000001000000}"/>
-    <hyperlink ref="K2" r:id="rId3" xr:uid="{00000000-0004-0000-0A00-000002000000}"/>
-    <hyperlink ref="K5" r:id="rId4" xr:uid="{00000000-0004-0000-0A00-000003000000}"/>
-    <hyperlink ref="K6" r:id="rId5" xr:uid="{00000000-0004-0000-0A00-000004000000}"/>
+    <hyperlink ref="K3" r:id="rId1"/>
+    <hyperlink ref="K4" r:id="rId2"/>
+    <hyperlink ref="K2" r:id="rId3"/>
+    <hyperlink ref="K5" r:id="rId4"/>
+    <hyperlink ref="K6" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId6"/>
@@ -3765,10 +3782,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:P24"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Q24"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="Q15" sqref="Q15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3784,9 +3803,10 @@
     <col min="12" max="12" width="30.7109375" style="1" customWidth="1"/>
     <col min="13" max="15" width="25.7109375" style="1" customWidth="1"/>
     <col min="16" max="16" width="110.7109375" style="1" customWidth="1"/>
+    <col min="17" max="17" width="26.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -3835,8 +3855,11 @@
       <c r="P1" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q1" s="2" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>30</v>
       </c>
@@ -3883,7 +3906,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>109</v>
       </c>
@@ -3931,7 +3954,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>148</v>
       </c>
@@ -3979,7 +4002,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>176</v>
       </c>
@@ -4026,7 +4049,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>177</v>
       </c>
@@ -4074,7 +4097,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>178</v>
       </c>
@@ -4122,7 +4145,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>252</v>
       </c>
@@ -4170,7 +4193,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>255</v>
       </c>
@@ -4218,7 +4241,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>312</v>
       </c>
@@ -4266,7 +4289,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>387</v>
       </c>
@@ -4313,7 +4336,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>389</v>
       </c>
@@ -4360,7 +4383,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>423</v>
       </c>
@@ -4407,56 +4430,110 @@
         <v>114</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="2" t="s">
+        <v>424</v>
+      </c>
+      <c r="C14" s="21" t="s">
+        <v>459</v>
+      </c>
+      <c r="D14" s="21" t="s">
+        <v>460</v>
+      </c>
+      <c r="E14" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="F14" s="14" t="s">
+        <v>253</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="H14" s="21" t="s">
+        <v>425</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="J14" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L14" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="M14" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="N14" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="O14" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="P14" s="23" t="s">
+        <v>461</v>
+      </c>
+      <c r="Q14" s="22" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P15" s="22"/>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="P16" s="22"/>
+    </row>
+    <row r="17" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B17" s="1"/>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="P17" s="20"/>
+    </row>
+    <row r="18" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B18" s="1"/>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B19" s="1"/>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B20" s="1"/>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B21" s="1"/>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B22" s="1"/>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B23" s="1"/>
     </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B24" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="P4" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
-    <hyperlink ref="P13" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
-    <hyperlink ref="P12" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
-    <hyperlink ref="P9" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
-    <hyperlink ref="P10" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
-    <hyperlink ref="P8" r:id="rId6" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
-    <hyperlink ref="P3" r:id="rId7" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
-    <hyperlink ref="P5" r:id="rId8" xr:uid="{00000000-0004-0000-0100-000007000000}"/>
-    <hyperlink ref="P2" r:id="rId9" xr:uid="{00000000-0004-0000-0100-000008000000}"/>
-    <hyperlink ref="P7" r:id="rId10" xr:uid="{00000000-0004-0000-0100-000009000000}"/>
-    <hyperlink ref="P11" r:id="rId11" xr:uid="{00000000-0004-0000-0100-00000A000000}"/>
-    <hyperlink ref="P6" r:id="rId12" xr:uid="{5192888D-8205-4B4C-B83F-C46360DCAAD8}"/>
+    <hyperlink ref="P4" r:id="rId1"/>
+    <hyperlink ref="P13" r:id="rId2"/>
+    <hyperlink ref="P12" r:id="rId3"/>
+    <hyperlink ref="P9" r:id="rId4"/>
+    <hyperlink ref="P10" r:id="rId5"/>
+    <hyperlink ref="P8" r:id="rId6"/>
+    <hyperlink ref="P3" r:id="rId7"/>
+    <hyperlink ref="P5" r:id="rId8"/>
+    <hyperlink ref="P2" r:id="rId9"/>
+    <hyperlink ref="P7" r:id="rId10"/>
+    <hyperlink ref="P11" r:id="rId11"/>
+    <hyperlink ref="P6" r:id="rId12"/>
+    <hyperlink ref="P14" r:id="rId13"/>
+    <hyperlink ref="Q14" r:id="rId14"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId13"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" r:id="rId15"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -4879,12 +4956,12 @@
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="S2" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
-    <hyperlink ref="S3" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
-    <hyperlink ref="S4" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
-    <hyperlink ref="S5" r:id="rId4" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
-    <hyperlink ref="S6" r:id="rId5" xr:uid="{00000000-0004-0000-0200-000004000000}"/>
-    <hyperlink ref="S7" r:id="rId6" xr:uid="{00000000-0004-0000-0200-000005000000}"/>
+    <hyperlink ref="S2" r:id="rId1"/>
+    <hyperlink ref="S3" r:id="rId2"/>
+    <hyperlink ref="S4" r:id="rId3"/>
+    <hyperlink ref="S5" r:id="rId4"/>
+    <hyperlink ref="S6" r:id="rId5"/>
+    <hyperlink ref="S7" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId7"/>
@@ -4892,7 +4969,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -5011,14 +5088,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="P2" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
+    <hyperlink ref="P2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -5321,13 +5398,13 @@
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="L2" r:id="rId1" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
-    <hyperlink ref="L5" r:id="rId2" xr:uid="{00000000-0004-0000-0400-000001000000}"/>
-    <hyperlink ref="L3" r:id="rId3" xr:uid="{00000000-0004-0000-0400-000002000000}"/>
-    <hyperlink ref="L6" r:id="rId4" xr:uid="{00000000-0004-0000-0400-000003000000}"/>
-    <hyperlink ref="L4" r:id="rId5" xr:uid="{00000000-0004-0000-0400-000004000000}"/>
-    <hyperlink ref="L7" r:id="rId6" xr:uid="{00000000-0004-0000-0400-000005000000}"/>
-    <hyperlink ref="L8" r:id="rId7" xr:uid="{C4AAA317-109D-4D9B-B5C9-67E54B2DF332}"/>
+    <hyperlink ref="L2" r:id="rId1"/>
+    <hyperlink ref="L5" r:id="rId2"/>
+    <hyperlink ref="L3" r:id="rId3"/>
+    <hyperlink ref="L6" r:id="rId4"/>
+    <hyperlink ref="L4" r:id="rId5"/>
+    <hyperlink ref="L7" r:id="rId6"/>
+    <hyperlink ref="L8" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId8"/>
@@ -5335,7 +5412,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -5504,15 +5581,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="P2" r:id="rId1" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
-    <hyperlink ref="P3" r:id="rId2" xr:uid="{00000000-0004-0000-0500-000001000000}"/>
+    <hyperlink ref="P2" r:id="rId1"/>
+    <hyperlink ref="P3" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -5712,14 +5789,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="M2" r:id="rId1" xr:uid="{00000000-0004-0000-0600-000000000000}"/>
+    <hyperlink ref="M2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -5895,15 +5972,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="Q2" r:id="rId1" xr:uid="{00000000-0004-0000-0700-000000000000}"/>
-    <hyperlink ref="Q3" r:id="rId2" xr:uid="{C629D676-045C-4851-83EF-DA670A6A6AA7}"/>
+    <hyperlink ref="Q2" r:id="rId1"/>
+    <hyperlink ref="Q3" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -5996,7 +6073,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="L2" r:id="rId1" xr:uid="{00000000-0004-0000-0800-000000000000}"/>
+    <hyperlink ref="L2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>